<commit_message>
Adicionado string de conexao e paginas do site finalizadas
</commit_message>
<xml_diff>
--- a/Modelagem/ModelagemBanco.xlsx
+++ b/Modelagem/ModelagemBanco.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CTTarde\Desktop\Eschechola\StreamTV-NETCore\Modelagem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\Git\StreamTV-NETCore\Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF5BAB0-732F-4C4F-8CBD-14718E3F317B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="23">
   <si>
     <t>Cliente</t>
   </si>
@@ -81,12 +82,24 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Contato</t>
+  </si>
+  <si>
+    <t>Id_Contato</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Problema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,7 +116,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,8 +147,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -158,11 +177,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -186,14 +218,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,11 +507,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B14" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,9 +519,10 @@
     <col min="1" max="1" width="48.42578125" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -497,65 +532,83 @@
       <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adicionar televisão com videos feito, falta testes
</commit_message>
<xml_diff>
--- a/Modelagem/ModelagemBanco.xlsx
+++ b/Modelagem/ModelagemBanco.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\Git\StreamTV-NETCore\Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF5BAB0-732F-4C4F-8CBD-14718E3F317B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616405DD-6D88-4B6F-8BFC-25537662BC01}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21480" yWindow="-30" windowWidth="19440" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Cliente</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Problema</t>
+  </si>
+  <si>
+    <t>Codigo</t>
   </si>
 </sst>
 </file>
@@ -511,7 +514,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B13:B14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +585,9 @@
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="C5" s="13" t="s">
         <v>16</v>
       </c>

</xml_diff>